<commit_message>
Mise à jour todolist
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t>Objectifs</t>
   </si>
@@ -24,6 +24,9 @@
     <t xml:space="preserve">Site de suivies, des collectes et distributions des dons pour les sinistrés</t>
   </si>
   <si>
+    <t xml:space="preserve">Partie 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Base de données</t>
   </si>
   <si>
@@ -211,6 +214,144 @@
   </si>
   <si>
     <t xml:space="preserve">Mettre des vrais données depuis la base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partie 2</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Tâche</t>
+  </si>
+  <si>
+    <t>Priorité</t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faire un table achat (avec colonne pourcentage)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">À faire</t>
+  </si>
+  <si>
+    <t>Backend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fonction de recuperation des frais d'achat</t>
+  </si>
+  <si>
+    <t>Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page de modification du % de frais</t>
+  </si>
+  <si>
+    <t>Achat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creer la table achat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Champs: id, ville_id, besoin_id, montant, pourcentage, montant_total, date_achat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verification du dons argents avant achat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calcul montant total avec frais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deduction auto du don argent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Message d'erreur si argent insuffisant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filtrer achats par ville</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page de saisi achat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vue </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liste des achats filtrables par ville</t>
+  </si>
+  <si>
+    <t>Simulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fonction simulation dispatch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calcul besoins satisfaits apres simulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calcul dons restants apres simulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bouton "Simuler"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Affichage tableau resultat simulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bouton "Valider"  pour insert dispatch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Besoins restants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calcul besoin total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calcul besoin satisfait</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calcul besoin restant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tableau des besoins restants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bouton "Acheter" par besoin</t>
+  </si>
+  <si>
+    <t>Recapitulatif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requete total besoins (SUM quantite × prix_unitaire)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requête total satisfaits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requête total restants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page récapitulatif</t>
+  </si>
+  <si>
+    <t>FrontEnd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bouton "Actualiser" en Ajax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requête AJAX refresh données</t>
+  </si>
+  <si>
+    <t>UX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Affichage cartes (Total / Satisfait / Restant)</t>
   </si>
 </sst>
 </file>
@@ -237,12 +378,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor theme="9" tint="-0.249977111117893"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -263,13 +410,15 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="9" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -768,15 +917,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A47" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="23.421875"/>
-    <col customWidth="1" min="2" max="2" width="14.7109375"/>
-    <col customWidth="1" min="3" max="3" width="36.00390625"/>
+    <col customWidth="1" min="2" max="2" width="16.140625"/>
+    <col customWidth="1" min="3" max="3" width="76.140625"/>
     <col customWidth="1" min="5" max="5" width="21.00390625"/>
     <col customWidth="1" min="6" max="6" width="14.28125"/>
     <col customWidth="1" min="8" max="8" width="27.7109375"/>
@@ -799,44 +948,12 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" ht="14.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
-      <c r="AA4" s="2"/>
-      <c r="AB4" s="2"/>
-      <c r="AC4" s="2"/>
-      <c r="AD4" s="2"/>
-      <c r="AE4" s="2"/>
-      <c r="AF4" s="2"/>
-      <c r="AG4" s="2"/>
-      <c r="AH4" s="2"/>
+    <row r="4" ht="18.75">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
     </row>
     <row r="5" ht="18.75">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1"/>
@@ -845,492 +962,1081 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" ht="18.75">
-      <c r="A7" s="1" t="s">
+    <row r="7" ht="14.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
+      <c r="AH7" s="3"/>
+    </row>
+    <row r="8" ht="18.75">
+      <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="E7" s="1" t="s">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" ht="18.75">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" ht="18.75">
+      <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" ht="14.25">
-      <c r="C8" t="s">
+      <c r="B10" s="1"/>
+      <c r="E10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" ht="14.25">
-      <c r="C9" t="s">
+    </row>
+    <row r="11" ht="14.25">
+      <c r="C11" t="s">
         <v>6</v>
       </c>
-      <c r="F9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" ht="18.75">
-      <c r="A11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="E11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>10</v>
+      <c r="F11" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12" ht="14.25">
       <c r="C12" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>5</v>
-      </c>
-      <c r="I12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" ht="18.75">
+      <c r="A14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="13" ht="14.25">
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" t="s">
-        <v>7</v>
-      </c>
-      <c r="I13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" ht="14.25">
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="I14" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="15" ht="14.25">
       <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" t="s">
         <v>14</v>
-      </c>
-      <c r="I15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" ht="18.75">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" ht="18.75">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="E17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="18" ht="14.25">
       <c r="C18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" ht="14.25">
-      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" ht="18.75">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" ht="18.75">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="F19" t="s">
-        <v>19</v>
-      </c>
-      <c r="I19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" ht="14.25">
-      <c r="C20" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" t="s">
-        <v>21</v>
-      </c>
-      <c r="I20" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="21" ht="14.25">
       <c r="C21" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="F21" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="I21" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" ht="14.25">
       <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24" t="s">
         <v>26</v>
       </c>
-      <c r="F22" t="s">
+    </row>
+    <row r="25" ht="14.25">
+      <c r="C25" t="s">
         <v>27</v>
       </c>
-      <c r="I22" t="s">
+      <c r="F25" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="23" ht="14.25">
-      <c r="F23" t="s">
+      <c r="I25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" ht="14.25">
-      <c r="F24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" s="2" customFormat="1" ht="15">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="27" ht="18.75">
-      <c r="A27" s="1" t="s">
+    <row r="26" ht="14.25">
+      <c r="F26" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="1" t="s">
+    </row>
+    <row r="27" ht="14.25">
+      <c r="F27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" s="3" customFormat="1" ht="15">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="30" ht="18.75">
+      <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" ht="16.5">
-      <c r="A28" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B28" s="4" t="s">
+      <c r="G30" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C28" t="s">
+    </row>
+    <row r="31" ht="16.5">
+      <c r="A31" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E28">
+      <c r="C31" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31">
         <v>9</v>
       </c>
-      <c r="F28" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" ht="16.5">
-      <c r="A29" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B29" s="4" t="s">
+      <c r="F31" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="4" t="s">
+    </row>
+    <row r="32" ht="16.5">
+      <c r="A32" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E29" s="4">
+      <c r="C32" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="5">
         <v>8</v>
       </c>
-      <c r="F29" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G29" s="5">
+      <c r="F32" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G32" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="30" ht="16.5">
-      <c r="A30" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="4" t="s">
+    <row r="33" ht="16.5">
+      <c r="A33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="4">
+      <c r="C33" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E33" s="5">
         <v>8</v>
       </c>
-      <c r="F30" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G30" s="5">
+      <c r="F33" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G33" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="31" ht="14.25">
-      <c r="A31" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31" t="s">
-        <v>37</v>
-      </c>
-      <c r="C31" t="s">
+    <row r="34" ht="14.25">
+      <c r="A34" t="s">
         <v>46</v>
       </c>
-      <c r="E31">
+      <c r="B34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34">
         <v>7</v>
       </c>
-      <c r="F31" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G31" s="5">
+      <c r="F34" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G34" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="32" ht="14.25">
-      <c r="A32" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" s="4" t="s">
+    <row r="35" ht="14.25">
+      <c r="A35" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" s="5">
+        <v>10</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E32" s="4">
+      <c r="G35" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" ht="14.25">
+      <c r="A36" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" s="5">
         <v>10</v>
       </c>
-      <c r="F32" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G32" s="5">
+      <c r="F36" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G36" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="33" ht="14.25">
-      <c r="A33" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E33" s="4">
+    <row r="37" ht="14.25">
+      <c r="A37" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37" s="5">
+        <v>7</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G37" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" ht="14.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" ht="14.25">
+      <c r="A39" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" t="s">
+        <v>55</v>
+      </c>
+      <c r="E39" s="5">
         <v>10</v>
       </c>
-      <c r="F33" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G33" s="5">
+      <c r="F39" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G39" s="6">
         <v>1</v>
-      </c>
-    </row>
-    <row r="34" ht="14.25">
-      <c r="A34" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E34" s="4">
-        <v>7</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G34" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" ht="14.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-    </row>
-    <row r="36" ht="14.25">
-      <c r="A36" t="s">
-        <v>52</v>
-      </c>
-      <c r="B36" t="s">
-        <v>53</v>
-      </c>
-      <c r="C36" t="s">
-        <v>54</v>
-      </c>
-      <c r="E36" s="4">
-        <v>10</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G36" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" ht="14.25">
-      <c r="A37" t="s">
-        <v>52</v>
-      </c>
-      <c r="B37" t="s">
-        <v>53</v>
-      </c>
-      <c r="C37" t="s">
-        <v>55</v>
-      </c>
-      <c r="E37" s="4">
-        <v>10</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G37" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" ht="14.25">
-      <c r="A38" t="s">
-        <v>56</v>
-      </c>
-      <c r="B38" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38" t="s">
-        <v>57</v>
-      </c>
-      <c r="E38">
-        <v>4</v>
-      </c>
-      <c r="F38" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="40" ht="14.25">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B40" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" t="s">
+        <v>56</v>
+      </c>
+      <c r="E40" s="5">
+        <v>10</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G40" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" ht="14.25">
+      <c r="A41" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41" t="s">
         <v>58</v>
       </c>
-      <c r="C40" t="s">
-        <v>59</v>
-      </c>
-      <c r="E40">
-        <v>5</v>
-      </c>
-      <c r="F40" t="s">
-        <v>39</v>
-      </c>
-      <c r="G40" s="5">
-        <v>0.92000000000000004</v>
-      </c>
-    </row>
-    <row r="42" ht="14.25">
-      <c r="A42" t="s">
-        <v>45</v>
-      </c>
-      <c r="B42" t="s">
-        <v>60</v>
-      </c>
-      <c r="C42" t="s">
-        <v>61</v>
-      </c>
-      <c r="E42">
+      <c r="E41">
         <v>4</v>
       </c>
-      <c r="F42" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G42" s="5">
-        <v>1</v>
+      <c r="F41" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="43" ht="14.25">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B43" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" t="s">
         <v>60</v>
-      </c>
-      <c r="C43" t="s">
-        <v>62</v>
       </c>
       <c r="E43">
         <v>5</v>
       </c>
-      <c r="F43" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G43" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" ht="14.25">
-      <c r="A44" t="s">
-        <v>53</v>
-      </c>
-      <c r="B44" t="s">
-        <v>53</v>
-      </c>
-      <c r="C44" t="s">
-        <v>63</v>
-      </c>
-      <c r="E44">
+      <c r="F43" t="s">
+        <v>40</v>
+      </c>
+      <c r="G43" s="6">
+        <v>0.92000000000000004</v>
+      </c>
+    </row>
+    <row r="45" ht="14.25">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" t="s">
+        <v>62</v>
+      </c>
+      <c r="E45">
         <v>4</v>
       </c>
-      <c r="F44" t="s">
-        <v>42</v>
-      </c>
-      <c r="G44" s="5">
+      <c r="F45" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G45" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="46" ht="14.25">
       <c r="A46" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B46" t="s">
+        <v>61</v>
+      </c>
+      <c r="C46" t="s">
+        <v>63</v>
+      </c>
+      <c r="E46">
+        <v>5</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G46" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" ht="14.25">
+      <c r="A47" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" t="s">
+        <v>64</v>
+      </c>
+      <c r="E47">
+        <v>4</v>
+      </c>
+      <c r="F47" t="s">
+        <v>43</v>
+      </c>
+      <c r="G47" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" ht="14.25">
+      <c r="A49" t="s">
         <v>53</v>
       </c>
-      <c r="C46" t="s">
-        <v>64</v>
-      </c>
-      <c r="E46">
+      <c r="B49" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49" t="s">
+        <v>65</v>
+      </c>
+      <c r="E49">
         <v>7</v>
       </c>
-      <c r="F46" t="s">
-        <v>42</v>
-      </c>
-      <c r="G46" s="5">
+      <c r="F49" t="s">
+        <v>43</v>
+      </c>
+      <c r="G49" s="6">
         <v>1</v>
+      </c>
+    </row>
+    <row r="51" ht="14.25">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+      <c r="O51" s="3"/>
+      <c r="P51" s="3"/>
+      <c r="Q51" s="3"/>
+      <c r="R51" s="3"/>
+      <c r="S51" s="3"/>
+      <c r="T51" s="3"/>
+      <c r="U51" s="3"/>
+      <c r="V51" s="3"/>
+      <c r="W51" s="3"/>
+      <c r="X51" s="3"/>
+      <c r="Y51" s="3"/>
+      <c r="Z51" s="3"/>
+      <c r="AA51" s="3"/>
+      <c r="AB51" s="3"/>
+      <c r="AC51" s="3"/>
+      <c r="AD51" s="3"/>
+      <c r="AE51" s="3"/>
+      <c r="AF51" s="3"/>
+      <c r="AG51" s="3"/>
+      <c r="AH51" s="3"/>
+      <c r="AI51" s="3"/>
+      <c r="AJ51" s="3"/>
+    </row>
+    <row r="53" ht="18.75">
+      <c r="A53" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="56" ht="14.25">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+      <c r="L56" s="3"/>
+      <c r="M56" s="3"/>
+      <c r="N56" s="3"/>
+      <c r="O56" s="3"/>
+      <c r="P56" s="3"/>
+      <c r="Q56" s="3"/>
+      <c r="R56" s="3"/>
+      <c r="S56" s="3"/>
+      <c r="T56" s="3"/>
+      <c r="U56" s="3"/>
+      <c r="V56" s="3"/>
+      <c r="W56" s="3"/>
+      <c r="X56" s="3"/>
+      <c r="Y56" s="3"/>
+      <c r="Z56" s="3"/>
+      <c r="AA56" s="3"/>
+      <c r="AB56" s="3"/>
+      <c r="AC56" s="3"/>
+      <c r="AD56" s="3"/>
+      <c r="AE56" s="3"/>
+      <c r="AF56" s="3"/>
+      <c r="AG56" s="3"/>
+      <c r="AH56" s="3"/>
+      <c r="AI56" s="3"/>
+      <c r="AJ56" s="3"/>
+    </row>
+    <row r="58" ht="18.75">
+      <c r="A58" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="59" ht="14.25">
+      <c r="A59" t="s">
+        <v>71</v>
+      </c>
+      <c r="B59" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59" t="s">
+        <v>72</v>
+      </c>
+      <c r="D59" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="60" ht="14.25">
+      <c r="A60" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B60" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" t="s">
+        <v>75</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="61" ht="14.25">
+      <c r="A61" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B61" t="s">
+        <v>76</v>
+      </c>
+      <c r="C61" t="s">
+        <v>77</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="62" ht="14.25">
+      <c r="D62" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="63" ht="14.25">
+      <c r="A63" t="s">
+        <v>78</v>
+      </c>
+      <c r="B63" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63" t="s">
+        <v>79</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="64" ht="14.25">
+      <c r="A64" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C64" t="s">
+        <v>80</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="65" ht="14.25">
+      <c r="A65" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B65" t="s">
+        <v>74</v>
+      </c>
+      <c r="C65" t="s">
+        <v>81</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="66" ht="14.25">
+      <c r="A66" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C66" t="s">
+        <v>82</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="67" ht="14.25">
+      <c r="A67" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C67" t="s">
+        <v>83</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="68" ht="14.25">
+      <c r="A68" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C68" t="s">
+        <v>84</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="69" ht="14.25">
+      <c r="A69" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C69" t="s">
+        <v>85</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="70" ht="14.25">
+      <c r="A70" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B70" t="s">
+        <v>54</v>
+      </c>
+      <c r="C70" t="s">
+        <v>86</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="71" ht="14.25">
+      <c r="A71" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B71" t="s">
+        <v>87</v>
+      </c>
+      <c r="C71" t="s">
+        <v>88</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72" ht="14.25">
+      <c r="D72" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="73" ht="14.25">
+      <c r="A73" t="s">
+        <v>89</v>
+      </c>
+      <c r="B73" t="s">
+        <v>74</v>
+      </c>
+      <c r="C73" t="s">
+        <v>90</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" ht="14.25">
+      <c r="A74" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C74" t="s">
+        <v>91</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" ht="14.25">
+      <c r="A75" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C75" t="s">
+        <v>92</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" ht="14.25">
+      <c r="A76" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B76" t="s">
+        <v>54</v>
+      </c>
+      <c r="C76" t="s">
+        <v>93</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="77" ht="14.25">
+      <c r="A77" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C77" t="s">
+        <v>94</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="78" ht="14.25">
+      <c r="A78" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B78" t="s">
+        <v>74</v>
+      </c>
+      <c r="C78" t="s">
+        <v>95</v>
+      </c>
+      <c r="D78" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="79" ht="14.25">
+      <c r="A79" s="7"/>
+      <c r="D79" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="80" ht="14.25">
+      <c r="A80" t="s">
+        <v>96</v>
+      </c>
+      <c r="B80" t="s">
+        <v>46</v>
+      </c>
+      <c r="C80" t="s">
+        <v>97</v>
+      </c>
+      <c r="D80" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="81" ht="14.25">
+      <c r="A81" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C81" t="s">
+        <v>98</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="82" ht="14.25">
+      <c r="A82" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C82" t="s">
+        <v>99</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="83" ht="14.25">
+      <c r="A83" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B83" t="s">
+        <v>54</v>
+      </c>
+      <c r="C83" t="s">
+        <v>100</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="84" ht="14.25">
+      <c r="A84" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B84" t="s">
+        <v>54</v>
+      </c>
+      <c r="C84" t="s">
+        <v>101</v>
+      </c>
+      <c r="D84" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="85" ht="14.25">
+      <c r="A85" s="7"/>
+      <c r="D85" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="86" ht="14.25">
+      <c r="A86" t="s">
+        <v>102</v>
+      </c>
+      <c r="B86" t="s">
+        <v>46</v>
+      </c>
+      <c r="C86" t="s">
+        <v>103</v>
+      </c>
+      <c r="D86" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="87" ht="14.25">
+      <c r="A87" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="88" ht="14.25">
+      <c r="A88" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C88" t="s">
+        <v>105</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="89" ht="14.25">
+      <c r="A89" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B89" t="s">
+        <v>54</v>
+      </c>
+      <c r="C89" t="s">
+        <v>106</v>
+      </c>
+      <c r="D89" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="90" ht="14.25">
+      <c r="A90" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B90" t="s">
+        <v>107</v>
+      </c>
+      <c r="C90" t="s">
+        <v>108</v>
+      </c>
+      <c r="D90" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="91" ht="14.25">
+      <c r="A91" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C91" t="s">
+        <v>109</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="92" ht="14.25">
+      <c r="A92" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B92" t="s">
+        <v>110</v>
+      </c>
+      <c r="C92" t="s">
+        <v>111</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
to do part 2
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -917,7 +917,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A47" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A70" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1610,9 +1610,12 @@
       <c r="D59" t="s">
         <v>73</v>
       </c>
+      <c r="F59" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="60" ht="14.25">
-      <c r="A60" s="7" t="s">
+      <c r="A60" s="5" t="s">
         <v>71</v>
       </c>
       <c r="B60" t="s">
@@ -1621,12 +1624,15 @@
       <c r="C60" t="s">
         <v>75</v>
       </c>
-      <c r="D60" s="7" t="s">
-        <v>73</v>
+      <c r="D60" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F60" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="61" ht="14.25">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="5" t="s">
         <v>71</v>
       </c>
       <c r="B61" t="s">
@@ -1635,12 +1641,15 @@
       <c r="C61" t="s">
         <v>77</v>
       </c>
-      <c r="D61" s="7" t="s">
-        <v>73</v>
+      <c r="D61" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F61" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="62" ht="14.25">
-      <c r="D62" s="7" t="s">
+      <c r="D62" s="5" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1654,26 +1663,32 @@
       <c r="C63" t="s">
         <v>79</v>
       </c>
-      <c r="D63" s="7" t="s">
-        <v>73</v>
+      <c r="D63" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F63" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="64" ht="14.25">
-      <c r="A64" s="7" t="s">
+      <c r="A64" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B64" s="7" t="s">
+      <c r="B64" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C64" t="s">
         <v>80</v>
       </c>
-      <c r="D64" s="7" t="s">
-        <v>73</v>
+      <c r="D64" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="65" ht="14.25">
-      <c r="A65" s="7" t="s">
+      <c r="A65" s="5" t="s">
         <v>78</v>
       </c>
       <c r="B65" t="s">
@@ -1682,68 +1697,83 @@
       <c r="C65" t="s">
         <v>81</v>
       </c>
-      <c r="D65" s="7" t="s">
-        <v>73</v>
+      <c r="D65" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F65" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="66" ht="14.25">
-      <c r="A66" s="7" t="s">
+      <c r="A66" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B66" s="7" t="s">
+      <c r="B66" s="5" t="s">
         <v>74</v>
       </c>
       <c r="C66" t="s">
         <v>82</v>
       </c>
-      <c r="D66" s="7" t="s">
-        <v>73</v>
+      <c r="D66" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="67" ht="14.25">
-      <c r="A67" s="7" t="s">
+      <c r="A67" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B67" s="7" t="s">
+      <c r="B67" s="5" t="s">
         <v>74</v>
       </c>
       <c r="C67" t="s">
         <v>83</v>
       </c>
-      <c r="D67" s="7" t="s">
-        <v>73</v>
+      <c r="D67" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="68" ht="14.25">
-      <c r="A68" s="7" t="s">
+      <c r="A68" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B68" s="5" t="s">
         <v>74</v>
       </c>
       <c r="C68" t="s">
         <v>84</v>
       </c>
-      <c r="D68" s="7" t="s">
-        <v>73</v>
+      <c r="D68" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="69" ht="14.25">
-      <c r="A69" s="7" t="s">
+      <c r="A69" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B69" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C69" t="s">
         <v>85</v>
       </c>
-      <c r="D69" s="7" t="s">
-        <v>73</v>
+      <c r="D69" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F69" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="70" ht="14.25">
-      <c r="A70" s="7" t="s">
+      <c r="A70" s="5" t="s">
         <v>78</v>
       </c>
       <c r="B70" t="s">
@@ -1752,12 +1782,15 @@
       <c r="C70" t="s">
         <v>86</v>
       </c>
-      <c r="D70" s="7" t="s">
-        <v>73</v>
+      <c r="D70" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="71" ht="14.25">
-      <c r="A71" s="7" t="s">
+      <c r="A71" s="5" t="s">
         <v>78</v>
       </c>
       <c r="B71" t="s">
@@ -1766,12 +1799,15 @@
       <c r="C71" t="s">
         <v>88</v>
       </c>
-      <c r="D71" s="7" t="s">
-        <v>73</v>
+      <c r="D71" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="72" ht="14.25">
-      <c r="D72" s="7" t="s">
+      <c r="D72" s="5" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1785,40 +1821,49 @@
       <c r="C73" t="s">
         <v>90</v>
       </c>
-      <c r="D73" s="7" t="s">
-        <v>73</v>
+      <c r="D73" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F73" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="74" ht="14.25">
-      <c r="A74" s="7" t="s">
+      <c r="A74" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B74" s="7" t="s">
+      <c r="B74" s="5" t="s">
         <v>74</v>
       </c>
       <c r="C74" t="s">
         <v>91</v>
       </c>
-      <c r="D74" s="7" t="s">
-        <v>73</v>
+      <c r="D74" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="75" ht="14.25">
-      <c r="A75" s="7" t="s">
+      <c r="A75" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B75" s="7" t="s">
+      <c r="B75" s="5" t="s">
         <v>74</v>
       </c>
       <c r="C75" t="s">
         <v>92</v>
       </c>
-      <c r="D75" s="7" t="s">
-        <v>73</v>
+      <c r="D75" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="76" ht="14.25">
-      <c r="A76" s="7" t="s">
+      <c r="A76" s="5" t="s">
         <v>89</v>
       </c>
       <c r="B76" t="s">
@@ -1827,26 +1872,32 @@
       <c r="C76" t="s">
         <v>93</v>
       </c>
-      <c r="D76" s="7" t="s">
-        <v>73</v>
+      <c r="D76" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F76" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="77" ht="14.25">
-      <c r="A77" s="7" t="s">
+      <c r="A77" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B77" s="7" t="s">
+      <c r="B77" s="5" t="s">
         <v>54</v>
       </c>
       <c r="C77" t="s">
         <v>94</v>
       </c>
-      <c r="D77" s="7" t="s">
-        <v>73</v>
+      <c r="D77" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F77" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="78" ht="14.25">
-      <c r="A78" s="7" t="s">
+      <c r="A78" s="5" t="s">
         <v>89</v>
       </c>
       <c r="B78" t="s">
@@ -1855,13 +1906,16 @@
       <c r="C78" t="s">
         <v>95</v>
       </c>
-      <c r="D78" s="7" t="s">
-        <v>73</v>
+      <c r="D78" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="79" ht="14.25">
-      <c r="A79" s="7"/>
-      <c r="D79" s="7" t="s">
+      <c r="A79" s="5"/>
+      <c r="D79" s="5" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1875,40 +1929,49 @@
       <c r="C80" t="s">
         <v>97</v>
       </c>
-      <c r="D80" s="7" t="s">
-        <v>73</v>
+      <c r="D80" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F80" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="81" ht="14.25">
-      <c r="A81" s="7" t="s">
+      <c r="A81" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B81" s="7" t="s">
+      <c r="B81" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C81" t="s">
         <v>98</v>
       </c>
-      <c r="D81" s="7" t="s">
-        <v>73</v>
+      <c r="D81" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="82" ht="14.25">
-      <c r="A82" s="7" t="s">
+      <c r="A82" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B82" s="7" t="s">
+      <c r="B82" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C82" t="s">
         <v>99</v>
       </c>
-      <c r="D82" s="7" t="s">
-        <v>73</v>
+      <c r="D82" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="83" ht="14.25">
-      <c r="A83" s="7" t="s">
+      <c r="A83" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B83" t="s">
@@ -1917,12 +1980,15 @@
       <c r="C83" t="s">
         <v>100</v>
       </c>
-      <c r="D83" s="7" t="s">
-        <v>73</v>
+      <c r="D83" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="84" ht="14.25">
-      <c r="A84" s="7" t="s">
+      <c r="A84" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B84" t="s">
@@ -1931,15 +1997,16 @@
       <c r="C84" t="s">
         <v>101</v>
       </c>
-      <c r="D84" s="7" t="s">
-        <v>73</v>
+      <c r="D84" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="85" ht="14.25">
-      <c r="A85" s="7"/>
-      <c r="D85" s="7" t="s">
-        <v>73</v>
-      </c>
+      <c r="A85" s="5"/>
+      <c r="D85" s="5"/>
     </row>
     <row r="86" ht="14.25">
       <c r="A86" t="s">
@@ -1951,40 +2018,49 @@
       <c r="C86" t="s">
         <v>103</v>
       </c>
-      <c r="D86" s="7" t="s">
-        <v>73</v>
+      <c r="D86" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F86" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="87" ht="14.25">
-      <c r="A87" s="7" t="s">
+      <c r="A87" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B87" s="7" t="s">
+      <c r="B87" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C87" s="7" t="s">
+      <c r="C87" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D87" s="7" t="s">
-        <v>73</v>
+      <c r="D87" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F87" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="88" ht="14.25">
-      <c r="A88" s="7" t="s">
+      <c r="A88" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B88" s="7" t="s">
+      <c r="B88" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C88" t="s">
         <v>105</v>
       </c>
-      <c r="D88" s="7" t="s">
-        <v>73</v>
+      <c r="D88" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F88" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="89" ht="14.25">
-      <c r="A89" s="7" t="s">
+      <c r="A89" s="5" t="s">
         <v>102</v>
       </c>
       <c r="B89" t="s">
@@ -1993,12 +2069,15 @@
       <c r="C89" t="s">
         <v>106</v>
       </c>
-      <c r="D89" s="7" t="s">
-        <v>73</v>
+      <c r="D89" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F89" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="90" ht="14.25">
-      <c r="A90" s="7" t="s">
+      <c r="A90" s="5" t="s">
         <v>102</v>
       </c>
       <c r="B90" t="s">
@@ -2007,26 +2086,32 @@
       <c r="C90" t="s">
         <v>108</v>
       </c>
-      <c r="D90" s="7" t="s">
-        <v>73</v>
+      <c r="D90" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F90" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="91" ht="14.25">
-      <c r="A91" s="7" t="s">
+      <c r="A91" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B91" s="7" t="s">
+      <c r="B91" s="5" t="s">
         <v>107</v>
       </c>
       <c r="C91" t="s">
         <v>109</v>
       </c>
-      <c r="D91" s="7" t="s">
-        <v>73</v>
+      <c r="D91" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F91" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="92" ht="14.25">
-      <c r="A92" s="7" t="s">
+      <c r="A92" s="5" t="s">
         <v>102</v>
       </c>
       <c r="B92" t="s">
@@ -2035,8 +2120,11 @@
       <c r="C92" t="s">
         <v>111</v>
       </c>
-      <c r="D92" s="7" t="s">
-        <v>73</v>
+      <c r="D92" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F92" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
base de données partie 2
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -410,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -418,7 +418,6 @@
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="9" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -917,7 +916,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A48" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1649,9 +1648,7 @@
       </c>
     </row>
     <row r="62" ht="14.25">
-      <c r="D62" s="5" t="s">
-        <v>73</v>
-      </c>
+      <c r="D62" s="5"/>
     </row>
     <row r="63" ht="14.25">
       <c r="A63" t="s">
@@ -1683,7 +1680,7 @@
       <c r="D64" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F64" s="7" t="s">
+      <c r="F64" s="5" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1717,7 +1714,7 @@
       <c r="D66" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F66" s="7" t="s">
+      <c r="F66" s="5" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1734,7 +1731,7 @@
       <c r="D67" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F67" s="7" t="s">
+      <c r="F67" s="5" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1751,7 +1748,7 @@
       <c r="D68" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F68" s="7" t="s">
+      <c r="F68" s="5" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1785,7 +1782,7 @@
       <c r="D70" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F70" s="7" t="s">
+      <c r="F70" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1802,14 +1799,12 @@
       <c r="D71" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F71" s="7" t="s">
+      <c r="F71" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="72" ht="14.25">
-      <c r="D72" s="5" t="s">
-        <v>73</v>
-      </c>
+      <c r="D72" s="5"/>
     </row>
     <row r="73" ht="14.25">
       <c r="A73" t="s">
@@ -1841,7 +1836,7 @@
       <c r="D74" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F74" s="7" t="s">
+      <c r="F74" s="5" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1858,7 +1853,7 @@
       <c r="D75" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F75" s="7" t="s">
+      <c r="F75" s="5" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1875,7 +1870,7 @@
       <c r="D76" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F76" s="7" t="s">
+      <c r="F76" s="5" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1909,7 +1904,7 @@
       <c r="D78" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F78" s="7" t="s">
+      <c r="F78" s="5" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1949,7 +1944,7 @@
       <c r="D81" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F81" s="7" t="s">
+      <c r="F81" s="5" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1966,7 +1961,7 @@
       <c r="D82" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F82" s="7" t="s">
+      <c r="F82" s="5" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1983,7 +1978,7 @@
       <c r="D83" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F83" s="7" t="s">
+      <c r="F83" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2000,7 +1995,7 @@
       <c r="D84" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F84" s="7" t="s">
+      <c r="F84" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2038,7 +2033,7 @@
       <c r="D87" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F87" s="7" t="s">
+      <c r="F87" s="5" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2055,7 +2050,7 @@
       <c r="D88" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F88" s="7" t="s">
+      <c r="F88" s="5" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Page de simulation dons
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t>Objectifs</t>
   </si>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t xml:space="preserve">Liste des achats filtrables par ville</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Simulation</t>
@@ -928,7 +931,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A60" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A59" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1689,7 +1692,9 @@
       <c r="F63" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G63" s="6"/>
+      <c r="G63" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="64" ht="14.25">
       <c r="A64" s="8" t="s">
@@ -1874,108 +1879,110 @@
       </c>
     </row>
     <row r="75" ht="14.25">
-      <c r="D75" s="5"/>
+      <c r="D75" s="9" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="76" ht="14.25">
       <c r="A76" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B76" t="s">
         <v>75</v>
       </c>
       <c r="C76" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>74</v>
       </c>
       <c r="F76" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="77" ht="14.25">
       <c r="A77" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>75</v>
       </c>
       <c r="C77" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F77" s="5" t="s">
-        <v>48</v>
+      <c r="F77" s="9" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="78" ht="14.25">
       <c r="A78" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>75</v>
       </c>
       <c r="C78" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F78" s="5" t="s">
-        <v>48</v>
+      <c r="F78" s="9" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="79" ht="14.25">
       <c r="A79" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B79" t="s">
         <v>54</v>
       </c>
       <c r="C79" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F79" s="5" t="s">
-        <v>48</v>
+      <c r="F79" s="9" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="80" ht="14.25">
       <c r="A80" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>54</v>
       </c>
       <c r="C80" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F80" t="s">
-        <v>48</v>
+      <c r="F80" s="9" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="81" ht="14.25">
       <c r="A81" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B81" t="s">
         <v>75</v>
       </c>
       <c r="C81" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F81" s="5" t="s">
-        <v>48</v>
+      <c r="F81" s="9" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="82" ht="14.25">
@@ -1984,13 +1991,13 @@
     </row>
     <row r="83" ht="14.25">
       <c r="A83" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B83" t="s">
         <v>46</v>
       </c>
       <c r="C83" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>74</v>
@@ -2001,13 +2008,13 @@
     </row>
     <row r="84" ht="14.25">
       <c r="A84" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B84" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C84" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>74</v>
@@ -2018,13 +2025,13 @@
     </row>
     <row r="85" ht="14.25">
       <c r="A85" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C85" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>74</v>
@@ -2035,13 +2042,13 @@
     </row>
     <row r="86" ht="14.25">
       <c r="A86" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B86" t="s">
         <v>54</v>
       </c>
       <c r="C86" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>74</v>
@@ -2052,13 +2059,13 @@
     </row>
     <row r="87" ht="14.25">
       <c r="A87" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B87" t="s">
         <v>54</v>
       </c>
       <c r="C87" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>74</v>
@@ -2073,13 +2080,13 @@
     </row>
     <row r="89" ht="14.25">
       <c r="A89" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B89" t="s">
         <v>46</v>
       </c>
       <c r="C89" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>74</v>
@@ -2090,13 +2097,13 @@
     </row>
     <row r="90" ht="14.25">
       <c r="A90" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D90" s="5" t="s">
         <v>74</v>
@@ -2107,13 +2114,13 @@
     </row>
     <row r="91" ht="14.25">
       <c r="A91" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B91" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C91" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D91" s="5" t="s">
         <v>74</v>
@@ -2124,13 +2131,13 @@
     </row>
     <row r="92" ht="14.25">
       <c r="A92" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B92" t="s">
         <v>54</v>
       </c>
       <c r="C92" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D92" s="5" t="s">
         <v>74</v>
@@ -2141,13 +2148,13 @@
     </row>
     <row r="93" ht="14.25">
       <c r="A93" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B93" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C93" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D93" s="5" t="s">
         <v>74</v>
@@ -2158,13 +2165,13 @@
     </row>
     <row r="94" ht="14.25">
       <c r="A94" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C94" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D94" s="5" t="s">
         <v>74</v>
@@ -2175,13 +2182,13 @@
     </row>
     <row r="95" ht="14.25">
       <c r="A95" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B95" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C95" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D95" s="5" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
Arrangement du theme des interfaces
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
     <t>Objectifs</t>
   </si>
@@ -364,6 +364,12 @@
   </si>
   <si>
     <t xml:space="preserve">Affichage cartes (Total / Satisfait / Restant)</t>
+  </si>
+  <si>
+    <t>UI/UX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design integrale des interfaces</t>
   </si>
 </sst>
 </file>
@@ -931,7 +937,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A59" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A78" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1899,6 +1905,9 @@
       <c r="F76" t="s">
         <v>43</v>
       </c>
+      <c r="G76" s="6">
+        <v>0.84999999999999998</v>
+      </c>
     </row>
     <row r="77" ht="14.25">
       <c r="A77" s="5" t="s">
@@ -1916,6 +1925,9 @@
       <c r="F77" s="9" t="s">
         <v>43</v>
       </c>
+      <c r="G77" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="78" ht="14.25">
       <c r="A78" s="5" t="s">
@@ -1933,6 +1945,9 @@
       <c r="F78" s="9" t="s">
         <v>43</v>
       </c>
+      <c r="G78" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="79" ht="14.25">
       <c r="A79" s="5" t="s">
@@ -1950,6 +1965,9 @@
       <c r="F79" s="9" t="s">
         <v>43</v>
       </c>
+      <c r="G79" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="80" ht="14.25">
       <c r="A80" s="5" t="s">
@@ -1967,6 +1985,9 @@
       <c r="F80" s="9" t="s">
         <v>43</v>
       </c>
+      <c r="G80" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="81" ht="14.25">
       <c r="A81" s="5" t="s">
@@ -1984,6 +2005,9 @@
       <c r="F81" s="9" t="s">
         <v>43</v>
       </c>
+      <c r="G81" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="82" ht="14.25">
       <c r="A82" s="5"/>
@@ -2195,6 +2219,23 @@
       </c>
       <c r="F95" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="97" ht="14.25">
+      <c r="A97" t="s">
+        <v>57</v>
+      </c>
+      <c r="B97" t="s">
+        <v>116</v>
+      </c>
+      <c r="C97" t="s">
+        <v>117</v>
+      </c>
+      <c r="D97" t="s">
+        <v>74</v>
+      </c>
+      <c r="F97" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correction bouton validation dispatch
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -937,7 +937,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A78" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A69" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2184,7 +2184,7 @@
         <v>74</v>
       </c>
       <c r="F93" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="94" ht="14.25">
@@ -2200,8 +2200,8 @@
       <c r="D94" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F94" t="s">
-        <v>48</v>
+      <c r="F94" s="9" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="95" ht="14.25">

</xml_diff>

<commit_message>
Correction de la barre d'indicateur des distribution des besoins
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -428,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -436,9 +436,6 @@
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="9" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -937,7 +934,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A69" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A74" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1676,26 +1673,25 @@
       </c>
     </row>
     <row r="62" ht="14.25">
-      <c r="A62" s="7"/>
-      <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
-      <c r="D62"/>
-      <c r="F62" s="7"/>
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="F62" s="5"/>
     </row>
     <row r="63" ht="14.25">
-      <c r="A63" s="8" t="s">
+      <c r="A63" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B63" s="8" t="s">
+      <c r="B63" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C63" s="8" t="s">
+      <c r="C63" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D63" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F63" s="8" t="s">
+      <c r="D63" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F63" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G63" s="6">
@@ -1703,19 +1699,19 @@
       </c>
     </row>
     <row r="64" ht="14.25">
-      <c r="A64" s="8" t="s">
+      <c r="A64" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="B64" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C64" s="8" t="s">
+      <c r="C64" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D64" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F64" s="8" t="s">
+      <c r="D64" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F64" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G64" s="6">
@@ -1885,7 +1881,7 @@
       </c>
     </row>
     <row r="75" ht="14.25">
-      <c r="D75" s="9" t="s">
+      <c r="D75" s="5" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1906,7 +1902,7 @@
         <v>43</v>
       </c>
       <c r="G76" s="6">
-        <v>0.84999999999999998</v>
+        <v>0.94999999999999996</v>
       </c>
     </row>
     <row r="77" ht="14.25">
@@ -1922,7 +1918,7 @@
       <c r="D77" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F77" s="9" t="s">
+      <c r="F77" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G77" s="6">
@@ -1942,7 +1938,7 @@
       <c r="D78" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F78" s="9" t="s">
+      <c r="F78" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G78" s="6">
@@ -1962,7 +1958,7 @@
       <c r="D79" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F79" s="9" t="s">
+      <c r="F79" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G79" s="6">
@@ -1982,7 +1978,7 @@
       <c r="D80" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F80" s="9" t="s">
+      <c r="F80" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G80" s="6">
@@ -2002,11 +1998,11 @@
       <c r="D81" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F81" s="9" t="s">
+      <c r="F81" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G81" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" ht="14.25">
@@ -2200,7 +2196,7 @@
       <c r="D94" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F94" s="9" t="s">
+      <c r="F94" s="5" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>